<commit_message>
Implementación del archivo donde se unifican los criterios de limpieza y tratamiento de datos
</commit_message>
<xml_diff>
--- a/Sample_Data/Raw/Criterios de busqueda/Criterios.xlsx
+++ b/Sample_Data/Raw/Criterios de busqueda/Criterios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paola\OneDrive\Documentos\Practicas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cceficiente-my.sharepoint.com/personal/jorge_ibanez_colombiacompra_gov_co/Documents/Solicitudes/Sample_Data/Raw/Criterios de busqueda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3435AD43-432B-40F5-9C76-C2C3D42B66EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{3435AD43-432B-40F5-9C76-C2C3D42B66EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0BBCF3E-1CB5-4444-B2CC-16F0EDB8810B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{61982D9F-CA56-45AD-8D3B-9C8996A4D756}"/>
+    <workbookView minimized="1" xWindow="888" yWindow="4476" windowWidth="12288" windowHeight="7776" xr2:uid="{61982D9F-CA56-45AD-8D3B-9C8996A4D756}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -979,7 +979,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1062,9 +1062,19 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96AE96C5-57CE-4761-9FCF-A2D79861DBE9}" name="Tabla1" displayName="Tabla1" ref="A1:C348" totalsRowShown="0">
-  <autoFilter ref="A1:C348" xr:uid="{96AE96C5-57CE-4761-9FCF-A2D79861DBE9}"/>
+  <autoFilter ref="A1:C348" xr:uid="{96AE96C5-57CE-4761-9FCF-A2D79861DBE9}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Combustible"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{02AA8EFA-CE3F-4516-B105-84939A487321}" name="Nombre_libro"/>
     <tableColumn id="2" xr3:uid="{B68B17D1-D352-4F5E-91AD-F57F0A409377}" name="Criterio"/>
@@ -1075,7 +1085,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1373,19 +1383,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25E9B68-1FBC-43C0-AE2B-5035E6E26EEF}">
   <dimension ref="A1:H348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A291" workbookViewId="0">
-      <selection activeCell="D348" sqref="D348"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C349" sqref="C349"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="67.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="67.109375" style="4" customWidth="1"/>
     <col min="4" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1396,7 +1406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1407,7 +1417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1418,7 +1428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1429,7 +1439,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1440,7 +1450,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1451,7 +1461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -1462,7 +1472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30">
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -1473,7 +1483,7 @@
         <v>851015</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1484,7 +1494,7 @@
         <v>851218</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1495,7 +1505,7 @@
         <v>851222</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1506,7 +1516,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1517,7 +1527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1528,7 +1538,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1539,7 +1549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1550,7 +1560,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -1561,7 +1571,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -1572,7 +1582,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1583,7 +1593,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -1594,7 +1604,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -1605,7 +1615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -1616,7 +1626,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1627,7 +1637,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -1638,7 +1648,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -1649,7 +1659,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
@@ -1660,7 +1670,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>21</v>
       </c>
@@ -1671,7 +1681,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
@@ -1682,7 +1692,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
@@ -1693,7 +1703,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>21</v>
       </c>
@@ -1704,7 +1714,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>21</v>
       </c>
@@ -1715,7 +1725,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>21</v>
       </c>
@@ -1726,7 +1736,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>21</v>
       </c>
@@ -1737,7 +1747,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>21</v>
       </c>
@@ -1748,7 +1758,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>21</v>
       </c>
@@ -1759,7 +1769,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>21</v>
       </c>
@@ -1770,7 +1780,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>21</v>
       </c>
@@ -1781,7 +1791,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>21</v>
       </c>
@@ -1792,7 +1802,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>21</v>
       </c>
@@ -1803,7 +1813,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>21</v>
       </c>
@@ -1814,7 +1824,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>21</v>
       </c>
@@ -1825,7 +1835,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>21</v>
       </c>
@@ -1836,7 +1846,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>21</v>
       </c>
@@ -1847,7 +1857,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>21</v>
       </c>
@@ -1858,7 +1868,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>44</v>
       </c>
@@ -1869,7 +1879,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>44</v>
       </c>
@@ -1880,7 +1890,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
@@ -1891,7 +1901,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>45</v>
       </c>
@@ -1902,7 +1912,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>45</v>
       </c>
@@ -1913,7 +1923,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>45</v>
       </c>
@@ -1924,7 +1934,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>45</v>
       </c>
@@ -1935,7 +1945,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>51</v>
       </c>
@@ -1946,7 +1956,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
@@ -1957,7 +1967,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>51</v>
       </c>
@@ -1968,7 +1978,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>51</v>
       </c>
@@ -1979,7 +1989,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>51</v>
       </c>
@@ -1990,7 +2000,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>53</v>
       </c>
@@ -2001,7 +2011,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>53</v>
       </c>
@@ -2012,7 +2022,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>53</v>
       </c>
@@ -2023,7 +2033,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>53</v>
       </c>
@@ -2034,7 +2044,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>53</v>
       </c>
@@ -2045,7 +2055,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>59</v>
       </c>
@@ -2056,7 +2066,7 @@
         <v>49000000</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>59</v>
       </c>
@@ -2067,7 +2077,7 @@
         <v>49130000</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>59</v>
       </c>
@@ -2078,7 +2088,7 @@
         <v>49140000</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>59</v>
       </c>
@@ -2089,7 +2099,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>59</v>
       </c>
@@ -2100,7 +2110,7 @@
         <v>49160000</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>59</v>
       </c>
@@ -2111,7 +2121,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>59</v>
       </c>
@@ -2122,7 +2132,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>59</v>
       </c>
@@ -2133,7 +2143,7 @@
         <v>49200000</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>59</v>
       </c>
@@ -2144,7 +2154,7 @@
         <v>49210000</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>59</v>
       </c>
@@ -2155,7 +2165,7 @@
         <v>49220000</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>63</v>
       </c>
@@ -2166,7 +2176,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>63</v>
       </c>
@@ -2177,7 +2187,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>63</v>
       </c>
@@ -2188,7 +2198,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>63</v>
       </c>
@@ -2199,7 +2209,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>68</v>
       </c>
@@ -2210,7 +2220,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>68</v>
       </c>
@@ -2221,7 +2231,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>68</v>
       </c>
@@ -2232,7 +2242,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>68</v>
       </c>
@@ -2243,7 +2253,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>68</v>
       </c>
@@ -2254,7 +2264,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>68</v>
       </c>
@@ -2265,7 +2275,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>68</v>
       </c>
@@ -2276,7 +2286,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>76</v>
       </c>
@@ -2287,7 +2297,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>76</v>
       </c>
@@ -2298,7 +2308,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>76</v>
       </c>
@@ -2309,7 +2319,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>76</v>
       </c>
@@ -2320,7 +2330,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>76</v>
       </c>
@@ -2331,7 +2341,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>76</v>
       </c>
@@ -2342,7 +2352,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>83</v>
       </c>
@@ -2353,7 +2363,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>83</v>
       </c>
@@ -2364,7 +2374,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>83</v>
       </c>
@@ -2375,7 +2385,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>83</v>
       </c>
@@ -2386,7 +2396,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>83</v>
       </c>
@@ -2397,7 +2407,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>83</v>
       </c>
@@ -2408,7 +2418,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>83</v>
       </c>
@@ -2419,7 +2429,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>38</v>
       </c>
@@ -2430,7 +2440,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>38</v>
       </c>
@@ -2441,7 +2451,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>38</v>
       </c>
@@ -2452,7 +2462,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>38</v>
       </c>
@@ -2463,7 +2473,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>38</v>
       </c>
@@ -2474,7 +2484,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>38</v>
       </c>
@@ -2485,7 +2495,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>38</v>
       </c>
@@ -2496,7 +2506,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>98</v>
       </c>
@@ -2507,7 +2517,7 @@
         <v>49000000</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>98</v>
       </c>
@@ -2518,7 +2528,7 @@
         <v>49130000</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>98</v>
       </c>
@@ -2529,7 +2539,7 @@
         <v>49140000</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>98</v>
       </c>
@@ -2540,7 +2550,7 @@
         <v>49150000</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>98</v>
       </c>
@@ -2551,7 +2561,7 @@
         <v>49160000</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>98</v>
       </c>
@@ -2562,7 +2572,7 @@
         <v>49170000</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>98</v>
       </c>
@@ -2573,7 +2583,7 @@
         <v>49180000</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>98</v>
       </c>
@@ -2584,7 +2594,7 @@
         <v>49200000</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>98</v>
       </c>
@@ -2595,7 +2605,7 @@
         <v>49210000</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>98</v>
       </c>
@@ -2606,7 +2616,7 @@
         <v>49220000</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>99</v>
       </c>
@@ -2617,7 +2627,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>99</v>
       </c>
@@ -2628,7 +2638,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>99</v>
       </c>
@@ -2639,7 +2649,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>103</v>
       </c>
@@ -2650,7 +2660,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>105</v>
       </c>
@@ -2661,7 +2671,7 @@
         <v>49000000</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>106</v>
       </c>
@@ -2672,7 +2682,7 @@
         <v>49130000</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>107</v>
       </c>
@@ -2683,7 +2693,7 @@
         <v>49140000</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>108</v>
       </c>
@@ -2694,7 +2704,7 @@
         <v>49150000</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>109</v>
       </c>
@@ -2705,7 +2715,7 @@
         <v>49160000</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>110</v>
       </c>
@@ -2716,7 +2726,7 @@
         <v>49170000</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>111</v>
       </c>
@@ -2727,7 +2737,7 @@
         <v>49180000</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>112</v>
       </c>
@@ -2738,7 +2748,7 @@
         <v>49200000</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>113</v>
       </c>
@@ -2752,7 +2762,7 @@
         <v>84765</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>114</v>
       </c>
@@ -2763,7 +2773,7 @@
         <v>49220000</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>115</v>
       </c>
@@ -2774,7 +2784,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>117</v>
       </c>
@@ -2785,7 +2795,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>117</v>
       </c>
@@ -2796,7 +2806,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>117</v>
       </c>
@@ -2807,7 +2817,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>117</v>
       </c>
@@ -2818,7 +2828,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>117</v>
       </c>
@@ -2829,7 +2839,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>117</v>
       </c>
@@ -2840,7 +2850,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>117</v>
       </c>
@@ -2851,7 +2861,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>117</v>
       </c>
@@ -2862,7 +2872,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>117</v>
       </c>
@@ -2873,7 +2883,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>127</v>
       </c>
@@ -2884,7 +2894,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>127</v>
       </c>
@@ -2895,7 +2905,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>127</v>
       </c>
@@ -2906,7 +2916,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>127</v>
       </c>
@@ -2917,7 +2927,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>127</v>
       </c>
@@ -2928,7 +2938,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>127</v>
       </c>
@@ -2939,7 +2949,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>127</v>
       </c>
@@ -2950,7 +2960,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>127</v>
       </c>
@@ -2961,7 +2971,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>127</v>
       </c>
@@ -2972,7 +2982,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>127</v>
       </c>
@@ -2983,7 +2993,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>127</v>
       </c>
@@ -2994,7 +3004,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>127</v>
       </c>
@@ -3005,7 +3015,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>127</v>
       </c>
@@ -3016,7 +3026,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>127</v>
       </c>
@@ -3027,7 +3037,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>127</v>
       </c>
@@ -3038,7 +3048,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>127</v>
       </c>
@@ -3049,7 +3059,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>127</v>
       </c>
@@ -3060,7 +3070,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>127</v>
       </c>
@@ -3071,7 +3081,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>127</v>
       </c>
@@ -3082,7 +3092,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>127</v>
       </c>
@@ -3093,7 +3103,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>127</v>
       </c>
@@ -3104,7 +3114,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>127</v>
       </c>
@@ -3115,7 +3125,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>150</v>
       </c>
@@ -3126,7 +3136,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>150</v>
       </c>
@@ -3137,7 +3147,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>150</v>
       </c>
@@ -3148,7 +3158,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>150</v>
       </c>
@@ -3159,7 +3169,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>155</v>
       </c>
@@ -3170,7 +3180,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>155</v>
       </c>
@@ -3181,7 +3191,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>155</v>
       </c>
@@ -3192,7 +3202,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>155</v>
       </c>
@@ -3203,7 +3213,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>155</v>
       </c>
@@ -3214,7 +3224,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>161</v>
       </c>
@@ -3225,7 +3235,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>161</v>
       </c>
@@ -3236,7 +3246,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>161</v>
       </c>
@@ -3247,7 +3257,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>161</v>
       </c>
@@ -3258,7 +3268,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>161</v>
       </c>
@@ -3269,7 +3279,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>161</v>
       </c>
@@ -3280,7 +3290,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>161</v>
       </c>
@@ -3291,7 +3301,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
+    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>161</v>
       </c>
@@ -3302,7 +3312,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>161</v>
       </c>
@@ -3313,7 +3323,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>161</v>
       </c>
@@ -3324,7 +3334,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
+    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>161</v>
       </c>
@@ -3335,7 +3345,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
+    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>161</v>
       </c>
@@ -3346,7 +3356,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
+    <row r="179" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>161</v>
       </c>
@@ -3357,7 +3367,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
+    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>161</v>
       </c>
@@ -3368,7 +3378,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
+    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>161</v>
       </c>
@@ -3379,7 +3389,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>161</v>
       </c>
@@ -3390,7 +3400,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
+    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>161</v>
       </c>
@@ -3401,7 +3411,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
+    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>161</v>
       </c>
@@ -3412,7 +3422,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="185" spans="1:3">
+    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>161</v>
       </c>
@@ -3423,7 +3433,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
+    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>161</v>
       </c>
@@ -3434,7 +3444,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
+    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>161</v>
       </c>
@@ -3445,7 +3455,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
+    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>161</v>
       </c>
@@ -3456,7 +3466,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
+    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>161</v>
       </c>
@@ -3467,7 +3477,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="190" spans="1:3">
+    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>185</v>
       </c>
@@ -3478,7 +3488,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="191" spans="1:3">
+    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>185</v>
       </c>
@@ -3489,7 +3499,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
+    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>185</v>
       </c>
@@ -3500,7 +3510,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
+    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>185</v>
       </c>
@@ -3511,7 +3521,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
+    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>185</v>
       </c>
@@ -3522,7 +3532,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>185</v>
       </c>
@@ -3533,7 +3543,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
+    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>185</v>
       </c>
@@ -3544,7 +3554,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
+    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>185</v>
       </c>
@@ -3555,7 +3565,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="198" spans="1:3">
+    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>185</v>
       </c>
@@ -3566,7 +3576,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="199" spans="1:3">
+    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>185</v>
       </c>
@@ -3577,7 +3587,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="200" spans="1:3">
+    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>185</v>
       </c>
@@ -3588,7 +3598,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="201" spans="1:3">
+    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>185</v>
       </c>
@@ -3599,7 +3609,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="202" spans="1:3">
+    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>185</v>
       </c>
@@ -3610,7 +3620,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="203" spans="1:3">
+    <row r="203" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>185</v>
       </c>
@@ -3621,7 +3631,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="204" spans="1:3">
+    <row r="204" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>185</v>
       </c>
@@ -3632,7 +3642,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="205" spans="1:3">
+    <row r="205" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>185</v>
       </c>
@@ -3643,7 +3653,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="206" spans="1:3">
+    <row r="206" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>202</v>
       </c>
@@ -3654,7 +3664,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="207" spans="1:3">
+    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>202</v>
       </c>
@@ -3665,7 +3675,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="208" spans="1:3">
+    <row r="208" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>202</v>
       </c>
@@ -3676,7 +3686,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>202</v>
       </c>
@@ -3687,7 +3697,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>202</v>
       </c>
@@ -3698,7 +3708,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="211" spans="1:3">
+    <row r="211" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>202</v>
       </c>
@@ -3709,7 +3719,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>202</v>
       </c>
@@ -3720,7 +3730,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="213" spans="1:3">
+    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>202</v>
       </c>
@@ -3731,7 +3741,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="214" spans="1:3">
+    <row r="214" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>202</v>
       </c>
@@ -3742,7 +3752,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="215" spans="1:3">
+    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>202</v>
       </c>
@@ -3753,7 +3763,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="216" spans="1:3">
+    <row r="216" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>202</v>
       </c>
@@ -3764,7 +3774,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
+    <row r="217" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>202</v>
       </c>
@@ -3775,7 +3785,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="218" spans="1:3">
+    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>202</v>
       </c>
@@ -3786,7 +3796,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="219" spans="1:3">
+    <row r="219" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>202</v>
       </c>
@@ -3797,7 +3807,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="220" spans="1:3">
+    <row r="220" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>202</v>
       </c>
@@ -3808,7 +3818,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="221" spans="1:3">
+    <row r="221" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>202</v>
       </c>
@@ -3819,7 +3829,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="222" spans="1:3">
+    <row r="222" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>202</v>
       </c>
@@ -3830,7 +3840,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="223" spans="1:3">
+    <row r="223" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>204</v>
       </c>
@@ -3841,7 +3851,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="224" spans="1:3">
+    <row r="224" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>204</v>
       </c>
@@ -3852,7 +3862,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="225" spans="1:3">
+    <row r="225" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>204</v>
       </c>
@@ -3863,7 +3873,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="226" spans="1:3">
+    <row r="226" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>204</v>
       </c>
@@ -3874,7 +3884,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="227" spans="1:3">
+    <row r="227" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>204</v>
       </c>
@@ -3885,7 +3895,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="228" spans="1:3">
+    <row r="228" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>204</v>
       </c>
@@ -3896,7 +3906,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="229" spans="1:3">
+    <row r="229" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>211</v>
       </c>
@@ -3907,7 +3917,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="230" spans="1:3">
+    <row r="230" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>211</v>
       </c>
@@ -3918,7 +3928,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="231" spans="1:3">
+    <row r="231" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>211</v>
       </c>
@@ -3929,7 +3939,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="232" spans="1:3">
+    <row r="232" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>211</v>
       </c>
@@ -3940,7 +3950,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="233" spans="1:3">
+    <row r="233" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>211</v>
       </c>
@@ -3951,7 +3961,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="234" spans="1:3">
+    <row r="234" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>211</v>
       </c>
@@ -3962,7 +3972,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="235" spans="1:3">
+    <row r="235" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>218</v>
       </c>
@@ -3973,7 +3983,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="236" spans="1:3">
+    <row r="236" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>220</v>
       </c>
@@ -3984,7 +3994,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="237" spans="1:3">
+    <row r="237" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>220</v>
       </c>
@@ -3995,7 +4005,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="238" spans="1:3">
+    <row r="238" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>220</v>
       </c>
@@ -4006,7 +4016,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="239" spans="1:3">
+    <row r="239" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>220</v>
       </c>
@@ -4017,7 +4027,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="240" spans="1:3">
+    <row r="240" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>220</v>
       </c>
@@ -4028,7 +4038,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>226</v>
       </c>
@@ -4039,7 +4049,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>226</v>
       </c>
@@ -4050,7 +4060,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="243" spans="1:3">
+    <row r="243" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>226</v>
       </c>
@@ -4061,7 +4071,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>226</v>
       </c>
@@ -4072,7 +4082,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="245" spans="1:3">
+    <row r="245" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>226</v>
       </c>
@@ -4083,7 +4093,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="246" spans="1:3">
+    <row r="246" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>226</v>
       </c>
@@ -4094,7 +4104,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="247" spans="1:3">
+    <row r="247" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>226</v>
       </c>
@@ -4105,7 +4115,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="248" spans="1:3">
+    <row r="248" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>226</v>
       </c>
@@ -4116,7 +4126,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="249" spans="1:3">
+    <row r="249" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>226</v>
       </c>
@@ -4127,7 +4137,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="250" spans="1:3">
+    <row r="250" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>226</v>
       </c>
@@ -4138,7 +4148,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="251" spans="1:3">
+    <row r="251" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>226</v>
       </c>
@@ -4149,7 +4159,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="252" spans="1:3">
+    <row r="252" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>226</v>
       </c>
@@ -4160,7 +4170,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="253" spans="1:3">
+    <row r="253" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>226</v>
       </c>
@@ -4171,7 +4181,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="254" spans="1:3">
+    <row r="254" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>226</v>
       </c>
@@ -4182,7 +4192,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="255" spans="1:3">
+    <row r="255" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>226</v>
       </c>
@@ -4193,7 +4203,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="256" spans="1:3">
+    <row r="256" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>226</v>
       </c>
@@ -4204,7 +4214,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="257" spans="1:3">
+    <row r="257" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>226</v>
       </c>
@@ -4215,7 +4225,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="258" spans="1:3">
+    <row r="258" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>226</v>
       </c>
@@ -4226,7 +4236,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="259" spans="1:3">
+    <row r="259" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>226</v>
       </c>
@@ -4237,7 +4247,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="260" spans="1:3">
+    <row r="260" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>226</v>
       </c>
@@ -4248,7 +4258,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="261" spans="1:3">
+    <row r="261" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>226</v>
       </c>
@@ -4259,7 +4269,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="262" spans="1:3">
+    <row r="262" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>226</v>
       </c>
@@ -4270,7 +4280,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="263" spans="1:3">
+    <row r="263" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>226</v>
       </c>
@@ -4281,7 +4291,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="264" spans="1:3">
+    <row r="264" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>226</v>
       </c>
@@ -4292,7 +4302,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="265" spans="1:3">
+    <row r="265" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>226</v>
       </c>
@@ -4303,7 +4313,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="266" spans="1:3">
+    <row r="266" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>226</v>
       </c>
@@ -4314,7 +4324,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="267" spans="1:3">
+    <row r="267" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>226</v>
       </c>
@@ -4325,7 +4335,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="268" spans="1:3">
+    <row r="268" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>226</v>
       </c>
@@ -4336,7 +4346,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="269" spans="1:3">
+    <row r="269" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>226</v>
       </c>
@@ -4347,7 +4357,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="270" spans="1:3">
+    <row r="270" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>226</v>
       </c>
@@ -4358,7 +4368,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="271" spans="1:3">
+    <row r="271" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>226</v>
       </c>
@@ -4369,7 +4379,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="272" spans="1:3">
+    <row r="272" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>226</v>
       </c>
@@ -4380,7 +4390,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="273" spans="1:3">
+    <row r="273" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>226</v>
       </c>
@@ -4391,7 +4401,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="274" spans="1:3">
+    <row r="274" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>226</v>
       </c>
@@ -4402,7 +4412,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="275" spans="1:3">
+    <row r="275" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>226</v>
       </c>
@@ -4413,7 +4423,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="276" spans="1:3">
+    <row r="276" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>226</v>
       </c>
@@ -4424,7 +4434,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="277" spans="1:3">
+    <row r="277" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>226</v>
       </c>
@@ -4435,7 +4445,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="278" spans="1:3">
+    <row r="278" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>226</v>
       </c>
@@ -4446,7 +4456,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="279" spans="1:3">
+    <row r="279" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>226</v>
       </c>
@@ -4457,7 +4467,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="280" spans="1:3">
+    <row r="280" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>226</v>
       </c>
@@ -4468,7 +4478,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="281" spans="1:3">
+    <row r="281" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>226</v>
       </c>
@@ -4479,7 +4489,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="282" spans="1:3">
+    <row r="282" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>226</v>
       </c>
@@ -4490,7 +4500,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="283" spans="1:3">
+    <row r="283" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>226</v>
       </c>
@@ -4501,7 +4511,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="284" spans="1:3">
+    <row r="284" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>226</v>
       </c>
@@ -4512,7 +4522,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="285" spans="1:3">
+    <row r="285" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>226</v>
       </c>
@@ -4523,7 +4533,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="286" spans="1:3">
+    <row r="286" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>226</v>
       </c>
@@ -4534,7 +4544,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="287" spans="1:3">
+    <row r="287" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>226</v>
       </c>
@@ -4545,7 +4555,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="288" spans="1:3">
+    <row r="288" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>226</v>
       </c>
@@ -4556,7 +4566,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="289" spans="1:3">
+    <row r="289" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>226</v>
       </c>
@@ -4567,7 +4577,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="290" spans="1:3">
+    <row r="290" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>226</v>
       </c>
@@ -4578,7 +4588,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="291" spans="1:3">
+    <row r="291" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>226</v>
       </c>
@@ -4589,7 +4599,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="292" spans="1:3">
+    <row r="292" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>226</v>
       </c>
@@ -4600,7 +4610,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="293" spans="1:3">
+    <row r="293" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>226</v>
       </c>
@@ -4611,7 +4621,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="294" spans="1:3">
+    <row r="294" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>277</v>
       </c>
@@ -4622,7 +4632,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="295" spans="1:3">
+    <row r="295" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>277</v>
       </c>
@@ -4633,7 +4643,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="296" spans="1:3">
+    <row r="296" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>277</v>
       </c>
@@ -4644,7 +4654,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="297" spans="1:3">
+    <row r="297" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>281</v>
       </c>
@@ -4655,7 +4665,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="298" spans="1:3">
+    <row r="298" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>281</v>
       </c>
@@ -4666,7 +4676,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="299" spans="1:3">
+    <row r="299" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>281</v>
       </c>
@@ -4677,7 +4687,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="300" spans="1:3">
+    <row r="300" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>281</v>
       </c>
@@ -4688,7 +4698,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="301" spans="1:3">
+    <row r="301" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>281</v>
       </c>
@@ -4699,7 +4709,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="302" spans="1:3">
+    <row r="302" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>281</v>
       </c>
@@ -4710,7 +4720,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="303" spans="1:3">
+    <row r="303" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>281</v>
       </c>
@@ -4721,7 +4731,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="304" spans="1:3">
+    <row r="304" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>281</v>
       </c>
@@ -4732,7 +4742,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="305" spans="1:3">
+    <row r="305" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>281</v>
       </c>
@@ -4743,7 +4753,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="306" spans="1:3">
+    <row r="306" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>281</v>
       </c>
@@ -4754,7 +4764,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="307" spans="1:3">
+    <row r="307" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>281</v>
       </c>
@@ -4765,7 +4775,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="308" spans="1:3">
+    <row r="308" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>281</v>
       </c>
@@ -4776,7 +4786,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="309" spans="1:3">
+    <row r="309" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>281</v>
       </c>
@@ -4787,7 +4797,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="310" spans="1:3">
+    <row r="310" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>281</v>
       </c>
@@ -4798,7 +4808,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="311" spans="1:3">
+    <row r="311" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>295</v>
       </c>
@@ -4809,7 +4819,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="312" spans="1:3">
+    <row r="312" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>295</v>
       </c>
@@ -4820,7 +4830,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="313" spans="1:3">
+    <row r="313" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>295</v>
       </c>
@@ -4831,7 +4841,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="314" spans="1:3">
+    <row r="314" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>295</v>
       </c>
@@ -4842,7 +4852,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="315" spans="1:3">
+    <row r="315" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>295</v>
       </c>
@@ -4853,7 +4863,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="316" spans="1:3">
+    <row r="316" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>295</v>
       </c>
@@ -4864,7 +4874,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="317" spans="1:3">
+    <row r="317" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>295</v>
       </c>
@@ -4875,7 +4885,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="318" spans="1:3">
+    <row r="318" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>295</v>
       </c>
@@ -4886,7 +4896,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="319" spans="1:3">
+    <row r="319" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>295</v>
       </c>
@@ -4897,7 +4907,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="320" spans="1:3">
+    <row r="320" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>295</v>
       </c>
@@ -4908,7 +4918,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="321" spans="1:3">
+    <row r="321" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>295</v>
       </c>
@@ -4919,7 +4929,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="322" spans="1:3">
+    <row r="322" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>295</v>
       </c>
@@ -4930,7 +4940,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="323" spans="1:3">
+    <row r="323" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>295</v>
       </c>
@@ -4941,7 +4951,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="324" spans="1:3">
+    <row r="324" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>295</v>
       </c>
@@ -4952,7 +4962,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="325" spans="1:3">
+    <row r="325" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>296</v>
       </c>
@@ -4963,7 +4973,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="326" spans="1:3">
+    <row r="326" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>296</v>
       </c>
@@ -4974,7 +4984,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="327" spans="1:3">
+    <row r="327" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>296</v>
       </c>
@@ -4985,7 +4995,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="328" spans="1:3">
+    <row r="328" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>296</v>
       </c>
@@ -4996,7 +5006,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="329" spans="1:3">
+    <row r="329" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>296</v>
       </c>
@@ -5007,7 +5017,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="330" spans="1:3">
+    <row r="330" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>296</v>
       </c>
@@ -5018,7 +5028,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="331" spans="1:3">
+    <row r="331" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>296</v>
       </c>
@@ -5029,7 +5039,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="332" spans="1:3">
+    <row r="332" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>296</v>
       </c>
@@ -5040,7 +5050,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="333" spans="1:3">
+    <row r="333" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>296</v>
       </c>
@@ -5051,7 +5061,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="334" spans="1:3">
+    <row r="334" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>296</v>
       </c>
@@ -5062,7 +5072,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="335" spans="1:3">
+    <row r="335" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>296</v>
       </c>
@@ -5073,7 +5083,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="336" spans="1:3">
+    <row r="336" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>296</v>
       </c>
@@ -5084,7 +5094,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="337" spans="1:3">
+    <row r="337" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>296</v>
       </c>
@@ -5095,7 +5105,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="338" spans="1:3">
+    <row r="338" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>296</v>
       </c>
@@ -5106,7 +5116,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="339" spans="1:3">
+    <row r="339" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>311</v>
       </c>
@@ -5117,7 +5127,7 @@
         <v>49000000</v>
       </c>
     </row>
-    <row r="340" spans="1:3">
+    <row r="340" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>311</v>
       </c>
@@ -5128,7 +5138,7 @@
         <v>49130000</v>
       </c>
     </row>
-    <row r="341" spans="1:3">
+    <row r="341" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>311</v>
       </c>
@@ -5139,7 +5149,7 @@
         <v>49140000</v>
       </c>
     </row>
-    <row r="342" spans="1:3">
+    <row r="342" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>311</v>
       </c>
@@ -5150,7 +5160,7 @@
         <v>49150000</v>
       </c>
     </row>
-    <row r="343" spans="1:3">
+    <row r="343" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>311</v>
       </c>
@@ -5161,7 +5171,7 @@
         <v>49160000</v>
       </c>
     </row>
-    <row r="344" spans="1:3">
+    <row r="344" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>311</v>
       </c>
@@ -5172,7 +5182,7 @@
         <v>49170000</v>
       </c>
     </row>
-    <row r="345" spans="1:3">
+    <row r="345" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>311</v>
       </c>
@@ -5183,7 +5193,7 @@
         <v>49180000</v>
       </c>
     </row>
-    <row r="346" spans="1:3">
+    <row r="346" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>311</v>
       </c>
@@ -5194,7 +5204,7 @@
         <v>49200000</v>
       </c>
     </row>
-    <row r="347" spans="1:3">
+    <row r="347" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>311</v>
       </c>
@@ -5205,7 +5215,7 @@
         <v>49210000</v>
       </c>
     </row>
-    <row r="348" spans="1:3">
+    <row r="348" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>311</v>
       </c>
@@ -5246,25 +5256,25 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>

</xml_diff>